<commit_message>
Updated product backlog & created sprint backlog
Did work.
</commit_message>
<xml_diff>
--- a/Product Backlog.xlsx
+++ b/Product Backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Team 47 Product Backlog</t>
   </si>
@@ -30,9 +30,6 @@
     <t>Adjust Estimate</t>
   </si>
   <si>
-    <t>Register &amp; Login Page</t>
-  </si>
-  <si>
     <t>Admin Account</t>
   </si>
   <si>
@@ -70,13 +67,28 @@
   </si>
   <si>
     <t>Total:</t>
+  </si>
+  <si>
+    <t>Welcome Page</t>
+  </si>
+  <si>
+    <t>Register Page</t>
+  </si>
+  <si>
+    <t>Login Page</t>
+  </si>
+  <si>
+    <t>Actual Login Implementation</t>
+  </si>
+  <si>
+    <t>Actual Register Implementation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -87,6 +99,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -115,10 +135,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -418,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -432,231 +452,291 @@
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+    <row r="1" spans="1:7" ht="18.75">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>1</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="1">
         <v>2</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C3">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D3">
         <f>B3+(B3*C3)</f>
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C4">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D14" si="0">B4+(B4*C4)</f>
-        <v>7.5</v>
+        <f>B4+(B4*C4)</f>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C5">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
-        <v>7.5</v>
+        <f>B5+(B5*C5)</f>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6">
         <v>7</v>
       </c>
-      <c r="B6">
-        <v>3</v>
-      </c>
       <c r="C6">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
-        <v>4.5</v>
+        <f>B6+(B6*C6)</f>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C7">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
-        <v>7.5</v>
+        <f>B7+(B7*C7)</f>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C8">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
-        <v>1.5</v>
+        <f t="shared" ref="D8:D18" si="0">B8+(B8*C8)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B9">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C9">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B10">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C10">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>22.5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B11">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C11">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>22.5</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B12">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="C12">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>22.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B13">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C13">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>22.5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B14">
         <v>15</v>
       </c>
       <c r="C14">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>22.5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:7">
-      <c r="A15" s="2" t="s">
-        <v>17</v>
+      <c r="A15" t="s">
+        <v>11</v>
       </c>
       <c r="B15">
-        <f>SUM(B3:B14)</f>
-        <v>114</v>
+        <v>15</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
       </c>
       <c r="D15">
-        <f>SUM(D3:D14)</f>
-        <v>171</v>
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18">
+        <v>15</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20">
+        <f>SUM(B3:B18)</f>
+        <v>143</v>
+      </c>
+      <c r="D20">
+        <f>SUM(D3:D18)</f>
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added priority column to product backlog
</commit_message>
<xml_diff>
--- a/Product Backlog.xlsx
+++ b/Product Backlog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Team 47 Product Backlog</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>Actual Register Implementation</t>
+  </si>
+  <si>
+    <t>Priority</t>
   </si>
 </sst>
 </file>
@@ -438,310 +441,361 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="47.42578125" customWidth="1"/>
-    <col min="2" max="2" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.42578125" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18.75">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2"/>
+    <row r="1" spans="1:8" ht="18.75">
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <v>1</v>
       </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>2</v>
       </c>
-      <c r="G2" s="1">
+      <c r="H2" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
+    <row r="3" spans="1:8">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>17</v>
       </c>
-      <c r="B3">
-        <v>5</v>
-      </c>
       <c r="C3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D3">
-        <f>B3+(B3*C3)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <f>C3+(C3*D3)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>19</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>7</v>
       </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
       <c r="D4">
-        <f>B4+(B4*C4)</f>
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <f>C4+(C4*D4)</f>
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
+    <row r="5" spans="1:8">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>20</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>10</v>
       </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
       <c r="D5">
-        <f>B5+(B5*C5)</f>
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <f>C5+(C5*D5)</f>
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
+    <row r="6" spans="1:8">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
         <v>18</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>7</v>
       </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
       <c r="D6">
-        <f>B6+(B6*C6)</f>
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <f>C6+(C6*D6)</f>
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
+    <row r="7" spans="1:8">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
         <v>21</v>
       </c>
-      <c r="B7">
+      <c r="C7">
         <v>10</v>
       </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
       <c r="D7">
-        <f>B7+(B7*C7)</f>
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <f>C7+(C7*D7)</f>
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
-      <c r="A8" t="s">
+    <row r="8" spans="1:8">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
         <v>4</v>
       </c>
-      <c r="B8">
-        <v>5</v>
-      </c>
       <c r="C8">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D8">
-        <f t="shared" ref="D8:D18" si="0">B8+(B8*C8)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ref="E8:E18" si="0">C8+(C8*D8)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
         <v>5</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
         <v>6</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>3</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
       <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
-      <c r="A11" t="s">
+    <row r="11" spans="1:8">
+      <c r="A11">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
         <v>8</v>
       </c>
-      <c r="B11">
-        <v>5</v>
-      </c>
       <c r="C11">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
         <v>9</v>
       </c>
-      <c r="B12">
+      <c r="C12">
         <v>1</v>
       </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
       <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
-      <c r="A13" t="s">
+    <row r="13" spans="1:8">
+      <c r="A13">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
         <v>7</v>
       </c>
-      <c r="B13">
+      <c r="C13">
         <v>10</v>
       </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
       <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
-      <c r="A14" t="s">
+    <row r="14" spans="1:8">
+      <c r="A14">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
         <v>10</v>
       </c>
-      <c r="B14">
-        <v>15</v>
-      </c>
       <c r="C14">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
         <v>11</v>
       </c>
-      <c r="B15">
-        <v>15</v>
-      </c>
       <c r="C15">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
         <v>12</v>
       </c>
-      <c r="B16">
-        <v>15</v>
-      </c>
       <c r="C16">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D16">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17">
+        <v>15</v>
+      </c>
+      <c r="B17" t="s">
         <v>13</v>
       </c>
-      <c r="B17">
-        <v>15</v>
-      </c>
       <c r="C17">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D17">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
-      <c r="A18" t="s">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18">
+        <v>16</v>
+      </c>
+      <c r="B18" t="s">
         <v>14</v>
       </c>
-      <c r="B18">
-        <v>15</v>
-      </c>
       <c r="C18">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="D18">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="B20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B20">
-        <f>SUM(B3:B18)</f>
+      <c r="C20">
+        <f>SUM(C3:C18)</f>
         <v>143</v>
       </c>
-      <c r="D20">
-        <f>SUM(D3:D18)</f>
+      <c r="E20">
+        <f>SUM(E3:E18)</f>
         <v>143</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>